<commit_message>
added recommendation engine code.
</commit_message>
<xml_diff>
--- a/moneymaker/stock_universe.xlsx
+++ b/moneymaker/stock_universe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jwilliams/PycharmProjects/moneymaker/moneymaker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D7F9A64-213B-F647-9117-6F1B913FF3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F84DD8-9C6C-FD42-A716-05BA4D813B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16520" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16520" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SPY" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="TDA_SCREEN" sheetId="5" r:id="rId4"/>
     <sheet name="TDA_SCREEN_SMALL" sheetId="6" r:id="rId5"/>
     <sheet name="WATCHLIST" sheetId="7" r:id="rId6"/>
+    <sheet name="Profit_Compare" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">TDA_SCREEN!$A$1:$G$492</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5786" uniqueCount="2522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5793" uniqueCount="2529">
   <si>
     <t>Apple Inc.</t>
   </si>
@@ -7608,13 +7609,37 @@
   </si>
   <si>
     <t>ETF</t>
+  </si>
+  <si>
+    <t>INVEST</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>IRATRADE</t>
+  </si>
+  <si>
+    <t>P/L Day - INVEST</t>
+  </si>
+  <si>
+    <t>P/L Day - IRATRADE</t>
+  </si>
+  <si>
+    <t>Balance - INVEST</t>
+  </si>
+  <si>
+    <t>Balance - IRATRADE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -7695,13 +7720,41 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -7713,12 +7766,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -7767,6 +7822,20 @@
     <xf numFmtId="10" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="14" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7780,9 +7849,11 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="Currency" xfId="4" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
     <cellStyle name="常规 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -16828,29 +16899,29 @@
       </c>
     </row>
     <row r="507" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A507" s="21"/>
-      <c r="B507" s="21"/>
-      <c r="C507" s="21"/>
-      <c r="D507" s="21"/>
-      <c r="E507" s="21"/>
+      <c r="A507" s="29"/>
+      <c r="B507" s="29"/>
+      <c r="C507" s="29"/>
+      <c r="D507" s="29"/>
+      <c r="E507" s="29"/>
       <c r="F507" s="1"/>
       <c r="G507" s="1"/>
     </row>
     <row r="508" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A508" s="21"/>
-      <c r="B508" s="21"/>
-      <c r="C508" s="21"/>
-      <c r="D508" s="21"/>
-      <c r="E508" s="21"/>
+      <c r="A508" s="29"/>
+      <c r="B508" s="29"/>
+      <c r="C508" s="29"/>
+      <c r="D508" s="29"/>
+      <c r="E508" s="29"/>
       <c r="F508" s="1"/>
       <c r="G508" s="1"/>
     </row>
     <row r="509" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A509" s="21"/>
-      <c r="B509" s="21"/>
-      <c r="C509" s="21"/>
-      <c r="D509" s="21"/>
-      <c r="E509" s="21"/>
+      <c r="A509" s="29"/>
+      <c r="B509" s="29"/>
+      <c r="C509" s="29"/>
+      <c r="D509" s="29"/>
+      <c r="E509" s="29"/>
       <c r="F509" s="1"/>
       <c r="G509" s="1"/>
     </row>
@@ -16864,21 +16935,21 @@
       <c r="G510" s="1"/>
     </row>
     <row r="511" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A511" s="20"/>
-      <c r="B511" s="20"/>
-      <c r="C511" s="20"/>
-      <c r="D511" s="20"/>
-      <c r="E511" s="20"/>
+      <c r="A511" s="28"/>
+      <c r="B511" s="28"/>
+      <c r="C511" s="28"/>
+      <c r="D511" s="28"/>
+      <c r="E511" s="28"/>
       <c r="F511" s="4"/>
       <c r="G511" s="4"/>
       <c r="H511" s="3"/>
     </row>
     <row r="512" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A512" s="20"/>
-      <c r="B512" s="20"/>
-      <c r="C512" s="20"/>
-      <c r="D512" s="20"/>
-      <c r="E512" s="20"/>
+      <c r="A512" s="28"/>
+      <c r="B512" s="28"/>
+      <c r="C512" s="28"/>
+      <c r="D512" s="28"/>
+      <c r="E512" s="28"/>
       <c r="F512" s="4"/>
       <c r="G512" s="4"/>
       <c r="H512" s="3"/>
@@ -16894,417 +16965,417 @@
       <c r="H513" s="3"/>
     </row>
     <row r="514" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A514" s="22"/>
-      <c r="B514" s="22"/>
-      <c r="C514" s="22"/>
-      <c r="D514" s="22"/>
-      <c r="E514" s="22"/>
+      <c r="A514" s="30"/>
+      <c r="B514" s="30"/>
+      <c r="C514" s="30"/>
+      <c r="D514" s="30"/>
+      <c r="E514" s="30"/>
     </row>
     <row r="515" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A515" s="22"/>
-      <c r="B515" s="22"/>
-      <c r="C515" s="22"/>
-      <c r="D515" s="22"/>
-      <c r="E515" s="22"/>
+      <c r="A515" s="30"/>
+      <c r="B515" s="30"/>
+      <c r="C515" s="30"/>
+      <c r="D515" s="30"/>
+      <c r="E515" s="30"/>
     </row>
     <row r="516" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A516" s="22"/>
-      <c r="B516" s="22"/>
-      <c r="C516" s="22"/>
-      <c r="D516" s="22"/>
-      <c r="E516" s="22"/>
+      <c r="A516" s="30"/>
+      <c r="B516" s="30"/>
+      <c r="C516" s="30"/>
+      <c r="D516" s="30"/>
+      <c r="E516" s="30"/>
     </row>
     <row r="517" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A517" s="22"/>
-      <c r="B517" s="22"/>
-      <c r="C517" s="22"/>
-      <c r="D517" s="22"/>
-      <c r="E517" s="22"/>
+      <c r="A517" s="30"/>
+      <c r="B517" s="30"/>
+      <c r="C517" s="30"/>
+      <c r="D517" s="30"/>
+      <c r="E517" s="30"/>
     </row>
     <row r="518" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A518" s="22"/>
-      <c r="B518" s="22"/>
-      <c r="C518" s="22"/>
-      <c r="D518" s="22"/>
-      <c r="E518" s="22"/>
+      <c r="A518" s="30"/>
+      <c r="B518" s="30"/>
+      <c r="C518" s="30"/>
+      <c r="D518" s="30"/>
+      <c r="E518" s="30"/>
     </row>
     <row r="519" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A519" s="22"/>
-      <c r="B519" s="22"/>
-      <c r="C519" s="22"/>
-      <c r="D519" s="22"/>
-      <c r="E519" s="22"/>
+      <c r="A519" s="30"/>
+      <c r="B519" s="30"/>
+      <c r="C519" s="30"/>
+      <c r="D519" s="30"/>
+      <c r="E519" s="30"/>
     </row>
     <row r="520" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A520" s="22"/>
-      <c r="B520" s="22"/>
-      <c r="C520" s="22"/>
-      <c r="D520" s="22"/>
-      <c r="E520" s="22"/>
+      <c r="A520" s="30"/>
+      <c r="B520" s="30"/>
+      <c r="C520" s="30"/>
+      <c r="D520" s="30"/>
+      <c r="E520" s="30"/>
     </row>
     <row r="521" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A521" s="22"/>
-      <c r="B521" s="22"/>
-      <c r="C521" s="22"/>
-      <c r="D521" s="22"/>
-      <c r="E521" s="22"/>
+      <c r="A521" s="30"/>
+      <c r="B521" s="30"/>
+      <c r="C521" s="30"/>
+      <c r="D521" s="30"/>
+      <c r="E521" s="30"/>
     </row>
     <row r="522" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A522" s="22"/>
-      <c r="B522" s="22"/>
-      <c r="C522" s="22"/>
-      <c r="D522" s="22"/>
-      <c r="E522" s="22"/>
+      <c r="A522" s="30"/>
+      <c r="B522" s="30"/>
+      <c r="C522" s="30"/>
+      <c r="D522" s="30"/>
+      <c r="E522" s="30"/>
     </row>
     <row r="523" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A523" s="22"/>
-      <c r="B523" s="22"/>
-      <c r="C523" s="22"/>
-      <c r="D523" s="22"/>
-      <c r="E523" s="22"/>
+      <c r="A523" s="30"/>
+      <c r="B523" s="30"/>
+      <c r="C523" s="30"/>
+      <c r="D523" s="30"/>
+      <c r="E523" s="30"/>
     </row>
     <row r="524" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A524" s="22"/>
-      <c r="B524" s="22"/>
-      <c r="C524" s="22"/>
-      <c r="D524" s="22"/>
-      <c r="E524" s="22"/>
+      <c r="A524" s="30"/>
+      <c r="B524" s="30"/>
+      <c r="C524" s="30"/>
+      <c r="D524" s="30"/>
+      <c r="E524" s="30"/>
     </row>
     <row r="525" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A525" s="22"/>
-      <c r="B525" s="22"/>
-      <c r="C525" s="22"/>
-      <c r="D525" s="22"/>
-      <c r="E525" s="22"/>
+      <c r="A525" s="30"/>
+      <c r="B525" s="30"/>
+      <c r="C525" s="30"/>
+      <c r="D525" s="30"/>
+      <c r="E525" s="30"/>
     </row>
     <row r="526" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A526" s="22"/>
-      <c r="B526" s="22"/>
-      <c r="C526" s="22"/>
-      <c r="D526" s="22"/>
-      <c r="E526" s="22"/>
+      <c r="A526" s="30"/>
+      <c r="B526" s="30"/>
+      <c r="C526" s="30"/>
+      <c r="D526" s="30"/>
+      <c r="E526" s="30"/>
     </row>
     <row r="527" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A527" s="22"/>
-      <c r="B527" s="22"/>
-      <c r="C527" s="22"/>
-      <c r="D527" s="22"/>
-      <c r="E527" s="22"/>
+      <c r="A527" s="30"/>
+      <c r="B527" s="30"/>
+      <c r="C527" s="30"/>
+      <c r="D527" s="30"/>
+      <c r="E527" s="30"/>
     </row>
     <row r="528" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A528" s="22"/>
-      <c r="B528" s="22"/>
-      <c r="C528" s="22"/>
-      <c r="D528" s="22"/>
-      <c r="E528" s="22"/>
+      <c r="A528" s="30"/>
+      <c r="B528" s="30"/>
+      <c r="C528" s="30"/>
+      <c r="D528" s="30"/>
+      <c r="E528" s="30"/>
     </row>
     <row r="529" spans="1:5" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A529" s="22"/>
-      <c r="B529" s="22"/>
-      <c r="C529" s="22"/>
-      <c r="D529" s="22"/>
-      <c r="E529" s="22"/>
+      <c r="A529" s="30"/>
+      <c r="B529" s="30"/>
+      <c r="C529" s="30"/>
+      <c r="D529" s="30"/>
+      <c r="E529" s="30"/>
     </row>
     <row r="530" spans="1:5" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A530" s="22"/>
-      <c r="B530" s="22"/>
-      <c r="C530" s="22"/>
-      <c r="D530" s="22"/>
-      <c r="E530" s="22"/>
+      <c r="A530" s="30"/>
+      <c r="B530" s="30"/>
+      <c r="C530" s="30"/>
+      <c r="D530" s="30"/>
+      <c r="E530" s="30"/>
     </row>
     <row r="531" spans="1:5" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A531" s="22"/>
-      <c r="B531" s="22"/>
-      <c r="C531" s="22"/>
-      <c r="D531" s="22"/>
-      <c r="E531" s="22"/>
+      <c r="A531" s="30"/>
+      <c r="B531" s="30"/>
+      <c r="C531" s="30"/>
+      <c r="D531" s="30"/>
+      <c r="E531" s="30"/>
     </row>
     <row r="532" spans="1:5" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A532" s="22"/>
-      <c r="B532" s="22"/>
-      <c r="C532" s="22"/>
-      <c r="D532" s="22"/>
-      <c r="E532" s="22"/>
+      <c r="A532" s="30"/>
+      <c r="B532" s="30"/>
+      <c r="C532" s="30"/>
+      <c r="D532" s="30"/>
+      <c r="E532" s="30"/>
     </row>
     <row r="533" spans="1:5" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A533" s="22"/>
-      <c r="B533" s="22"/>
-      <c r="C533" s="22"/>
-      <c r="D533" s="22"/>
-      <c r="E533" s="22"/>
+      <c r="A533" s="30"/>
+      <c r="B533" s="30"/>
+      <c r="C533" s="30"/>
+      <c r="D533" s="30"/>
+      <c r="E533" s="30"/>
     </row>
     <row r="534" spans="1:5" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A534" s="22"/>
-      <c r="B534" s="22"/>
-      <c r="C534" s="22"/>
-      <c r="D534" s="22"/>
-      <c r="E534" s="22"/>
+      <c r="A534" s="30"/>
+      <c r="B534" s="30"/>
+      <c r="C534" s="30"/>
+      <c r="D534" s="30"/>
+      <c r="E534" s="30"/>
     </row>
     <row r="535" spans="1:5" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A535" s="22"/>
-      <c r="B535" s="22"/>
-      <c r="C535" s="22"/>
-      <c r="D535" s="22"/>
-      <c r="E535" s="22"/>
+      <c r="A535" s="30"/>
+      <c r="B535" s="30"/>
+      <c r="C535" s="30"/>
+      <c r="D535" s="30"/>
+      <c r="E535" s="30"/>
     </row>
     <row r="536" spans="1:5" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A536" s="22"/>
-      <c r="B536" s="22"/>
-      <c r="C536" s="22"/>
-      <c r="D536" s="22"/>
-      <c r="E536" s="22"/>
+      <c r="A536" s="30"/>
+      <c r="B536" s="30"/>
+      <c r="C536" s="30"/>
+      <c r="D536" s="30"/>
+      <c r="E536" s="30"/>
     </row>
     <row r="537" spans="1:5" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A537" s="22"/>
-      <c r="B537" s="22"/>
-      <c r="C537" s="22"/>
-      <c r="D537" s="22"/>
-      <c r="E537" s="22"/>
+      <c r="A537" s="30"/>
+      <c r="B537" s="30"/>
+      <c r="C537" s="30"/>
+      <c r="D537" s="30"/>
+      <c r="E537" s="30"/>
     </row>
     <row r="538" spans="1:5" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A538" s="22"/>
-      <c r="B538" s="22"/>
-      <c r="C538" s="22"/>
-      <c r="D538" s="22"/>
-      <c r="E538" s="22"/>
+      <c r="A538" s="30"/>
+      <c r="B538" s="30"/>
+      <c r="C538" s="30"/>
+      <c r="D538" s="30"/>
+      <c r="E538" s="30"/>
     </row>
     <row r="539" spans="1:5" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A539" s="22"/>
-      <c r="B539" s="22"/>
-      <c r="C539" s="22"/>
-      <c r="D539" s="22"/>
-      <c r="E539" s="22"/>
+      <c r="A539" s="30"/>
+      <c r="B539" s="30"/>
+      <c r="C539" s="30"/>
+      <c r="D539" s="30"/>
+      <c r="E539" s="30"/>
     </row>
     <row r="540" spans="1:5" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A540" s="22"/>
-      <c r="B540" s="22"/>
-      <c r="C540" s="22"/>
-      <c r="D540" s="22"/>
-      <c r="E540" s="22"/>
+      <c r="A540" s="30"/>
+      <c r="B540" s="30"/>
+      <c r="C540" s="30"/>
+      <c r="D540" s="30"/>
+      <c r="E540" s="30"/>
     </row>
     <row r="541" spans="1:5" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A541" s="22"/>
-      <c r="B541" s="22"/>
-      <c r="C541" s="22"/>
-      <c r="D541" s="22"/>
-      <c r="E541" s="22"/>
+      <c r="A541" s="30"/>
+      <c r="B541" s="30"/>
+      <c r="C541" s="30"/>
+      <c r="D541" s="30"/>
+      <c r="E541" s="30"/>
     </row>
     <row r="542" spans="1:5" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A542" s="22"/>
-      <c r="B542" s="22"/>
-      <c r="C542" s="22"/>
-      <c r="D542" s="22"/>
-      <c r="E542" s="22"/>
+      <c r="A542" s="30"/>
+      <c r="B542" s="30"/>
+      <c r="C542" s="30"/>
+      <c r="D542" s="30"/>
+      <c r="E542" s="30"/>
     </row>
     <row r="543" spans="1:5" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A543" s="22"/>
-      <c r="B543" s="22"/>
-      <c r="C543" s="22"/>
-      <c r="D543" s="22"/>
-      <c r="E543" s="22"/>
+      <c r="A543" s="30"/>
+      <c r="B543" s="30"/>
+      <c r="C543" s="30"/>
+      <c r="D543" s="30"/>
+      <c r="E543" s="30"/>
     </row>
     <row r="544" spans="1:5" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A544" s="22"/>
-      <c r="B544" s="22"/>
-      <c r="C544" s="22"/>
-      <c r="D544" s="22"/>
-      <c r="E544" s="22"/>
+      <c r="A544" s="30"/>
+      <c r="B544" s="30"/>
+      <c r="C544" s="30"/>
+      <c r="D544" s="30"/>
+      <c r="E544" s="30"/>
     </row>
     <row r="545" spans="1:5" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A545" s="22"/>
-      <c r="B545" s="22"/>
-      <c r="C545" s="22"/>
-      <c r="D545" s="22"/>
-      <c r="E545" s="22"/>
+      <c r="A545" s="30"/>
+      <c r="B545" s="30"/>
+      <c r="C545" s="30"/>
+      <c r="D545" s="30"/>
+      <c r="E545" s="30"/>
     </row>
     <row r="546" spans="1:5" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A546" s="22"/>
-      <c r="B546" s="22"/>
-      <c r="C546" s="22"/>
-      <c r="D546" s="22"/>
-      <c r="E546" s="22"/>
+      <c r="A546" s="30"/>
+      <c r="B546" s="30"/>
+      <c r="C546" s="30"/>
+      <c r="D546" s="30"/>
+      <c r="E546" s="30"/>
     </row>
     <row r="547" spans="1:5" s="5" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A547" s="22"/>
-      <c r="B547" s="22"/>
-      <c r="C547" s="22"/>
-      <c r="D547" s="22"/>
-      <c r="E547" s="22"/>
+      <c r="A547" s="30"/>
+      <c r="B547" s="30"/>
+      <c r="C547" s="30"/>
+      <c r="D547" s="30"/>
+      <c r="E547" s="30"/>
     </row>
     <row r="548" spans="1:5" s="5" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A548" s="22"/>
-      <c r="B548" s="22"/>
-      <c r="C548" s="22"/>
-      <c r="D548" s="22"/>
-      <c r="E548" s="22"/>
+      <c r="A548" s="30"/>
+      <c r="B548" s="30"/>
+      <c r="C548" s="30"/>
+      <c r="D548" s="30"/>
+      <c r="E548" s="30"/>
     </row>
     <row r="549" spans="1:5" s="5" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A549" s="22"/>
-      <c r="B549" s="22"/>
-      <c r="C549" s="22"/>
-      <c r="D549" s="22"/>
-      <c r="E549" s="22"/>
+      <c r="A549" s="30"/>
+      <c r="B549" s="30"/>
+      <c r="C549" s="30"/>
+      <c r="D549" s="30"/>
+      <c r="E549" s="30"/>
     </row>
     <row r="550" spans="1:5" s="5" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A550" s="22"/>
-      <c r="B550" s="22"/>
-      <c r="C550" s="22"/>
-      <c r="D550" s="22"/>
-      <c r="E550" s="22"/>
+      <c r="A550" s="30"/>
+      <c r="B550" s="30"/>
+      <c r="C550" s="30"/>
+      <c r="D550" s="30"/>
+      <c r="E550" s="30"/>
     </row>
     <row r="551" spans="1:5" s="5" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A551" s="22"/>
-      <c r="B551" s="22"/>
-      <c r="C551" s="22"/>
-      <c r="D551" s="22"/>
-      <c r="E551" s="22"/>
+      <c r="A551" s="30"/>
+      <c r="B551" s="30"/>
+      <c r="C551" s="30"/>
+      <c r="D551" s="30"/>
+      <c r="E551" s="30"/>
     </row>
     <row r="552" spans="1:5" s="5" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A552" s="22"/>
-      <c r="B552" s="22"/>
-      <c r="C552" s="22"/>
-      <c r="D552" s="22"/>
-      <c r="E552" s="22"/>
+      <c r="A552" s="30"/>
+      <c r="B552" s="30"/>
+      <c r="C552" s="30"/>
+      <c r="D552" s="30"/>
+      <c r="E552" s="30"/>
     </row>
     <row r="553" spans="1:5" s="5" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A553" s="22"/>
-      <c r="B553" s="22"/>
-      <c r="C553" s="22"/>
-      <c r="D553" s="22"/>
-      <c r="E553" s="22"/>
+      <c r="A553" s="30"/>
+      <c r="B553" s="30"/>
+      <c r="C553" s="30"/>
+      <c r="D553" s="30"/>
+      <c r="E553" s="30"/>
     </row>
     <row r="554" spans="1:5" s="5" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A554" s="22"/>
-      <c r="B554" s="22"/>
-      <c r="C554" s="22"/>
-      <c r="D554" s="22"/>
-      <c r="E554" s="22"/>
+      <c r="A554" s="30"/>
+      <c r="B554" s="30"/>
+      <c r="C554" s="30"/>
+      <c r="D554" s="30"/>
+      <c r="E554" s="30"/>
     </row>
     <row r="555" spans="1:5" s="5" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A555" s="22"/>
-      <c r="B555" s="22"/>
-      <c r="C555" s="22"/>
-      <c r="D555" s="22"/>
-      <c r="E555" s="22"/>
+      <c r="A555" s="30"/>
+      <c r="B555" s="30"/>
+      <c r="C555" s="30"/>
+      <c r="D555" s="30"/>
+      <c r="E555" s="30"/>
     </row>
     <row r="556" spans="1:5" s="5" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A556" s="22"/>
-      <c r="B556" s="22"/>
-      <c r="C556" s="22"/>
-      <c r="D556" s="22"/>
-      <c r="E556" s="22"/>
+      <c r="A556" s="30"/>
+      <c r="B556" s="30"/>
+      <c r="C556" s="30"/>
+      <c r="D556" s="30"/>
+      <c r="E556" s="30"/>
     </row>
     <row r="557" spans="1:5" s="5" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A557" s="22"/>
-      <c r="B557" s="22"/>
-      <c r="C557" s="22"/>
-      <c r="D557" s="22"/>
-      <c r="E557" s="22"/>
+      <c r="A557" s="30"/>
+      <c r="B557" s="30"/>
+      <c r="C557" s="30"/>
+      <c r="D557" s="30"/>
+      <c r="E557" s="30"/>
     </row>
     <row r="558" spans="1:5" s="5" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A558" s="22"/>
-      <c r="B558" s="22"/>
-      <c r="C558" s="22"/>
-      <c r="D558" s="22"/>
-      <c r="E558" s="22"/>
+      <c r="A558" s="30"/>
+      <c r="B558" s="30"/>
+      <c r="C558" s="30"/>
+      <c r="D558" s="30"/>
+      <c r="E558" s="30"/>
     </row>
     <row r="559" spans="1:5" s="5" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A559" s="22"/>
-      <c r="B559" s="22"/>
-      <c r="C559" s="22"/>
-      <c r="D559" s="22"/>
-      <c r="E559" s="22"/>
+      <c r="A559" s="30"/>
+      <c r="B559" s="30"/>
+      <c r="C559" s="30"/>
+      <c r="D559" s="30"/>
+      <c r="E559" s="30"/>
     </row>
     <row r="560" spans="1:5" s="5" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A560" s="22"/>
-      <c r="B560" s="22"/>
-      <c r="C560" s="22"/>
-      <c r="D560" s="22"/>
-      <c r="E560" s="22"/>
+      <c r="A560" s="30"/>
+      <c r="B560" s="30"/>
+      <c r="C560" s="30"/>
+      <c r="D560" s="30"/>
+      <c r="E560" s="30"/>
     </row>
     <row r="561" spans="1:5" s="5" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A561" s="22"/>
-      <c r="B561" s="22"/>
-      <c r="C561" s="22"/>
-      <c r="D561" s="22"/>
-      <c r="E561" s="22"/>
+      <c r="A561" s="30"/>
+      <c r="B561" s="30"/>
+      <c r="C561" s="30"/>
+      <c r="D561" s="30"/>
+      <c r="E561" s="30"/>
     </row>
     <row r="562" spans="1:5" s="5" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A562" s="22"/>
-      <c r="B562" s="22"/>
-      <c r="C562" s="22"/>
-      <c r="D562" s="22"/>
-      <c r="E562" s="22"/>
+      <c r="A562" s="30"/>
+      <c r="B562" s="30"/>
+      <c r="C562" s="30"/>
+      <c r="D562" s="30"/>
+      <c r="E562" s="30"/>
     </row>
     <row r="563" spans="1:5" s="5" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A563" s="22"/>
-      <c r="B563" s="22"/>
-      <c r="C563" s="22"/>
-      <c r="D563" s="22"/>
-      <c r="E563" s="22"/>
+      <c r="A563" s="30"/>
+      <c r="B563" s="30"/>
+      <c r="C563" s="30"/>
+      <c r="D563" s="30"/>
+      <c r="E563" s="30"/>
     </row>
     <row r="564" spans="1:5" s="5" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A564" s="22"/>
-      <c r="B564" s="22"/>
-      <c r="C564" s="22"/>
-      <c r="D564" s="22"/>
-      <c r="E564" s="22"/>
+      <c r="A564" s="30"/>
+      <c r="B564" s="30"/>
+      <c r="C564" s="30"/>
+      <c r="D564" s="30"/>
+      <c r="E564" s="30"/>
     </row>
     <row r="565" spans="1:5" s="5" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A565" s="22"/>
-      <c r="B565" s="22"/>
-      <c r="C565" s="22"/>
-      <c r="D565" s="22"/>
-      <c r="E565" s="22"/>
+      <c r="A565" s="30"/>
+      <c r="B565" s="30"/>
+      <c r="C565" s="30"/>
+      <c r="D565" s="30"/>
+      <c r="E565" s="30"/>
     </row>
     <row r="566" spans="1:5" s="5" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A566" s="22"/>
-      <c r="B566" s="22"/>
-      <c r="C566" s="22"/>
-      <c r="D566" s="22"/>
-      <c r="E566" s="22"/>
+      <c r="A566" s="30"/>
+      <c r="B566" s="30"/>
+      <c r="C566" s="30"/>
+      <c r="D566" s="30"/>
+      <c r="E566" s="30"/>
     </row>
     <row r="567" spans="1:5" s="5" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A567" s="22"/>
-      <c r="B567" s="22"/>
-      <c r="C567" s="22"/>
-      <c r="D567" s="22"/>
-      <c r="E567" s="22"/>
+      <c r="A567" s="30"/>
+      <c r="B567" s="30"/>
+      <c r="C567" s="30"/>
+      <c r="D567" s="30"/>
+      <c r="E567" s="30"/>
     </row>
     <row r="568" spans="1:5" s="5" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A568" s="22"/>
-      <c r="B568" s="22"/>
-      <c r="C568" s="22"/>
-      <c r="D568" s="22"/>
-      <c r="E568" s="22"/>
+      <c r="A568" s="30"/>
+      <c r="B568" s="30"/>
+      <c r="C568" s="30"/>
+      <c r="D568" s="30"/>
+      <c r="E568" s="30"/>
     </row>
     <row r="569" spans="1:5" s="5" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A569" s="22"/>
-      <c r="B569" s="22"/>
-      <c r="C569" s="22"/>
-      <c r="D569" s="22"/>
-      <c r="E569" s="22"/>
+      <c r="A569" s="30"/>
+      <c r="B569" s="30"/>
+      <c r="C569" s="30"/>
+      <c r="D569" s="30"/>
+      <c r="E569" s="30"/>
     </row>
     <row r="570" spans="1:5" s="5" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A570" s="22"/>
-      <c r="B570" s="22"/>
-      <c r="C570" s="22"/>
-      <c r="D570" s="22"/>
-      <c r="E570" s="22"/>
+      <c r="A570" s="30"/>
+      <c r="B570" s="30"/>
+      <c r="C570" s="30"/>
+      <c r="D570" s="30"/>
+      <c r="E570" s="30"/>
     </row>
     <row r="571" spans="1:5" s="5" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A571" s="22"/>
-      <c r="B571" s="22"/>
-      <c r="C571" s="22"/>
-      <c r="D571" s="22"/>
-      <c r="E571" s="22"/>
+      <c r="A571" s="30"/>
+      <c r="B571" s="30"/>
+      <c r="C571" s="30"/>
+      <c r="D571" s="30"/>
+      <c r="E571" s="30"/>
     </row>
     <row r="572" spans="1:5" s="5" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A572" s="22"/>
-      <c r="B572" s="22"/>
-      <c r="C572" s="22"/>
-      <c r="D572" s="22"/>
-      <c r="E572" s="22"/>
+      <c r="A572" s="30"/>
+      <c r="B572" s="30"/>
+      <c r="C572" s="30"/>
+      <c r="D572" s="30"/>
+      <c r="E572" s="30"/>
     </row>
     <row r="573" spans="1:5" s="5" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A573" s="8"/>
@@ -17314,60 +17385,60 @@
       <c r="E573" s="8"/>
     </row>
     <row r="574" spans="1:5" s="5" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A574" s="23"/>
-      <c r="B574" s="23"/>
-      <c r="C574" s="23"/>
-      <c r="D574" s="23"/>
-      <c r="E574" s="23"/>
+      <c r="A574" s="31"/>
+      <c r="B574" s="31"/>
+      <c r="C574" s="31"/>
+      <c r="D574" s="31"/>
+      <c r="E574" s="31"/>
     </row>
     <row r="575" spans="1:5" s="5" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A575" s="23"/>
-      <c r="B575" s="23"/>
-      <c r="C575" s="23"/>
-      <c r="D575" s="23"/>
-      <c r="E575" s="23"/>
+      <c r="A575" s="31"/>
+      <c r="B575" s="31"/>
+      <c r="C575" s="31"/>
+      <c r="D575" s="31"/>
+      <c r="E575" s="31"/>
     </row>
     <row r="576" spans="1:5" s="5" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A576" s="23"/>
-      <c r="B576" s="23"/>
-      <c r="C576" s="23"/>
-      <c r="D576" s="23"/>
-      <c r="E576" s="23"/>
+      <c r="A576" s="31"/>
+      <c r="B576" s="31"/>
+      <c r="C576" s="31"/>
+      <c r="D576" s="31"/>
+      <c r="E576" s="31"/>
     </row>
     <row r="577" spans="1:7" s="5" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A577" s="23"/>
-      <c r="B577" s="23"/>
-      <c r="C577" s="23"/>
-      <c r="D577" s="23"/>
-      <c r="E577" s="23"/>
+      <c r="A577" s="31"/>
+      <c r="B577" s="31"/>
+      <c r="C577" s="31"/>
+      <c r="D577" s="31"/>
+      <c r="E577" s="31"/>
     </row>
     <row r="578" spans="1:7" s="5" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A578" s="23"/>
-      <c r="B578" s="23"/>
-      <c r="C578" s="23"/>
-      <c r="D578" s="23"/>
-      <c r="E578" s="23"/>
+      <c r="A578" s="31"/>
+      <c r="B578" s="31"/>
+      <c r="C578" s="31"/>
+      <c r="D578" s="31"/>
+      <c r="E578" s="31"/>
     </row>
     <row r="579" spans="1:7" s="5" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A579" s="23"/>
-      <c r="B579" s="23"/>
-      <c r="C579" s="23"/>
-      <c r="D579" s="23"/>
-      <c r="E579" s="23"/>
+      <c r="A579" s="31"/>
+      <c r="B579" s="31"/>
+      <c r="C579" s="31"/>
+      <c r="D579" s="31"/>
+      <c r="E579" s="31"/>
     </row>
     <row r="580" spans="1:7" s="5" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A580" s="23"/>
-      <c r="B580" s="23"/>
-      <c r="C580" s="23"/>
-      <c r="D580" s="23"/>
-      <c r="E580" s="23"/>
+      <c r="A580" s="31"/>
+      <c r="B580" s="31"/>
+      <c r="C580" s="31"/>
+      <c r="D580" s="31"/>
+      <c r="E580" s="31"/>
     </row>
     <row r="581" spans="1:7" s="5" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A581" s="23"/>
-      <c r="B581" s="23"/>
-      <c r="C581" s="23"/>
-      <c r="D581" s="23"/>
-      <c r="E581" s="23"/>
+      <c r="A581" s="31"/>
+      <c r="B581" s="31"/>
+      <c r="C581" s="31"/>
+      <c r="D581" s="31"/>
+      <c r="E581" s="31"/>
     </row>
     <row r="582" spans="1:7" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A582" s="10"/>
@@ -17377,74 +17448,74 @@
       <c r="E582" s="8"/>
     </row>
     <row r="583" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A583" s="22"/>
-      <c r="B583" s="22"/>
-      <c r="C583" s="22"/>
-      <c r="D583" s="22"/>
-      <c r="E583" s="22"/>
+      <c r="A583" s="30"/>
+      <c r="B583" s="30"/>
+      <c r="C583" s="30"/>
+      <c r="D583" s="30"/>
+      <c r="E583" s="30"/>
       <c r="F583" s="2"/>
       <c r="G583" s="2"/>
     </row>
     <row r="584" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A584" s="22"/>
-      <c r="B584" s="22"/>
-      <c r="C584" s="22"/>
-      <c r="D584" s="22"/>
-      <c r="E584" s="22"/>
+      <c r="A584" s="30"/>
+      <c r="B584" s="30"/>
+      <c r="C584" s="30"/>
+      <c r="D584" s="30"/>
+      <c r="E584" s="30"/>
       <c r="F584" s="2"/>
       <c r="G584" s="2"/>
     </row>
     <row r="585" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A585" s="22"/>
-      <c r="B585" s="22"/>
-      <c r="C585" s="22"/>
-      <c r="D585" s="22"/>
-      <c r="E585" s="22"/>
+      <c r="A585" s="30"/>
+      <c r="B585" s="30"/>
+      <c r="C585" s="30"/>
+      <c r="D585" s="30"/>
+      <c r="E585" s="30"/>
       <c r="F585" s="2"/>
       <c r="G585" s="2"/>
     </row>
     <row r="586" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A586" s="22"/>
-      <c r="B586" s="22"/>
-      <c r="C586" s="22"/>
-      <c r="D586" s="22"/>
-      <c r="E586" s="22"/>
+      <c r="A586" s="30"/>
+      <c r="B586" s="30"/>
+      <c r="C586" s="30"/>
+      <c r="D586" s="30"/>
+      <c r="E586" s="30"/>
       <c r="F586" s="2"/>
       <c r="G586" s="2"/>
     </row>
     <row r="587" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A587" s="22"/>
-      <c r="B587" s="22"/>
-      <c r="C587" s="22"/>
-      <c r="D587" s="22"/>
-      <c r="E587" s="22"/>
+      <c r="A587" s="30"/>
+      <c r="B587" s="30"/>
+      <c r="C587" s="30"/>
+      <c r="D587" s="30"/>
+      <c r="E587" s="30"/>
       <c r="F587" s="2"/>
       <c r="G587" s="2"/>
     </row>
     <row r="588" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A588" s="22"/>
-      <c r="B588" s="22"/>
-      <c r="C588" s="22"/>
-      <c r="D588" s="22"/>
-      <c r="E588" s="22"/>
+      <c r="A588" s="30"/>
+      <c r="B588" s="30"/>
+      <c r="C588" s="30"/>
+      <c r="D588" s="30"/>
+      <c r="E588" s="30"/>
       <c r="F588" s="2"/>
       <c r="G588" s="2"/>
     </row>
     <row r="589" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A589" s="22"/>
-      <c r="B589" s="22"/>
-      <c r="C589" s="22"/>
-      <c r="D589" s="22"/>
-      <c r="E589" s="22"/>
+      <c r="A589" s="30"/>
+      <c r="B589" s="30"/>
+      <c r="C589" s="30"/>
+      <c r="D589" s="30"/>
+      <c r="E589" s="30"/>
       <c r="F589" s="2"/>
       <c r="G589" s="2"/>
     </row>
     <row r="590" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A590" s="22"/>
-      <c r="B590" s="22"/>
-      <c r="C590" s="22"/>
-      <c r="D590" s="22"/>
-      <c r="E590" s="22"/>
+      <c r="A590" s="30"/>
+      <c r="B590" s="30"/>
+      <c r="C590" s="30"/>
+      <c r="D590" s="30"/>
+      <c r="E590" s="30"/>
       <c r="F590" s="2"/>
       <c r="G590" s="2"/>
     </row>
@@ -17458,83 +17529,83 @@
       <c r="G591" s="2"/>
     </row>
     <row r="592" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A592" s="22"/>
-      <c r="B592" s="22"/>
-      <c r="C592" s="22"/>
-      <c r="D592" s="22"/>
-      <c r="E592" s="22"/>
+      <c r="A592" s="30"/>
+      <c r="B592" s="30"/>
+      <c r="C592" s="30"/>
+      <c r="D592" s="30"/>
+      <c r="E592" s="30"/>
       <c r="F592" s="2"/>
       <c r="G592" s="2"/>
     </row>
     <row r="593" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A593" s="22"/>
-      <c r="B593" s="22"/>
-      <c r="C593" s="22"/>
-      <c r="D593" s="22"/>
-      <c r="E593" s="22"/>
+      <c r="A593" s="30"/>
+      <c r="B593" s="30"/>
+      <c r="C593" s="30"/>
+      <c r="D593" s="30"/>
+      <c r="E593" s="30"/>
     </row>
     <row r="594" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A594" s="22"/>
-      <c r="B594" s="22"/>
-      <c r="C594" s="22"/>
-      <c r="D594" s="22"/>
-      <c r="E594" s="22"/>
+      <c r="A594" s="30"/>
+      <c r="B594" s="30"/>
+      <c r="C594" s="30"/>
+      <c r="D594" s="30"/>
+      <c r="E594" s="30"/>
     </row>
     <row r="595" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A595" s="22"/>
-      <c r="B595" s="22"/>
-      <c r="C595" s="22"/>
-      <c r="D595" s="22"/>
-      <c r="E595" s="22"/>
+      <c r="A595" s="30"/>
+      <c r="B595" s="30"/>
+      <c r="C595" s="30"/>
+      <c r="D595" s="30"/>
+      <c r="E595" s="30"/>
     </row>
     <row r="596" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A596" s="22"/>
-      <c r="B596" s="22"/>
-      <c r="C596" s="22"/>
-      <c r="D596" s="22"/>
-      <c r="E596" s="22"/>
+      <c r="A596" s="30"/>
+      <c r="B596" s="30"/>
+      <c r="C596" s="30"/>
+      <c r="D596" s="30"/>
+      <c r="E596" s="30"/>
     </row>
     <row r="597" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A597" s="22"/>
-      <c r="B597" s="22"/>
-      <c r="C597" s="22"/>
-      <c r="D597" s="22"/>
-      <c r="E597" s="22"/>
+      <c r="A597" s="30"/>
+      <c r="B597" s="30"/>
+      <c r="C597" s="30"/>
+      <c r="D597" s="30"/>
+      <c r="E597" s="30"/>
     </row>
     <row r="598" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A598" s="22"/>
-      <c r="B598" s="22"/>
-      <c r="C598" s="22"/>
-      <c r="D598" s="22"/>
-      <c r="E598" s="22"/>
+      <c r="A598" s="30"/>
+      <c r="B598" s="30"/>
+      <c r="C598" s="30"/>
+      <c r="D598" s="30"/>
+      <c r="E598" s="30"/>
     </row>
     <row r="599" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A599" s="22"/>
-      <c r="B599" s="22"/>
-      <c r="C599" s="22"/>
-      <c r="D599" s="22"/>
-      <c r="E599" s="22"/>
+      <c r="A599" s="30"/>
+      <c r="B599" s="30"/>
+      <c r="C599" s="30"/>
+      <c r="D599" s="30"/>
+      <c r="E599" s="30"/>
     </row>
     <row r="600" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A600" s="22"/>
-      <c r="B600" s="22"/>
-      <c r="C600" s="22"/>
-      <c r="D600" s="22"/>
-      <c r="E600" s="22"/>
+      <c r="A600" s="30"/>
+      <c r="B600" s="30"/>
+      <c r="C600" s="30"/>
+      <c r="D600" s="30"/>
+      <c r="E600" s="30"/>
     </row>
     <row r="601" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A601" s="22"/>
-      <c r="B601" s="22"/>
-      <c r="C601" s="22"/>
-      <c r="D601" s="22"/>
-      <c r="E601" s="22"/>
+      <c r="A601" s="30"/>
+      <c r="B601" s="30"/>
+      <c r="C601" s="30"/>
+      <c r="D601" s="30"/>
+      <c r="E601" s="30"/>
     </row>
     <row r="602" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A602" s="22"/>
-      <c r="B602" s="22"/>
-      <c r="C602" s="22"/>
-      <c r="D602" s="22"/>
-      <c r="E602" s="22"/>
+      <c r="A602" s="30"/>
+      <c r="B602" s="30"/>
+      <c r="C602" s="30"/>
+      <c r="D602" s="30"/>
+      <c r="E602" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -21295,7 +21366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28814948-BB70-7547-AA2B-46C432DD5217}">
   <dimension ref="A1:G503"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A477" workbookViewId="0">
+    <sheetView topLeftCell="A477" workbookViewId="0">
       <selection activeCell="B488" sqref="B488"/>
     </sheetView>
   </sheetViews>
@@ -36202,4 +36273,293 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74AE2592-5FD4-204D-9AAA-B82BCF31AA88}">
+  <dimension ref="A1:G30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" style="27" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" style="27" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" style="27" customWidth="1"/>
+    <col min="7" max="7" width="25.5" style="27" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>2523</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>2522</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>2524</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>2525</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>2527</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>2526</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>2528</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="20">
+        <v>44994</v>
+      </c>
+      <c r="B2" s="24">
+        <f>(D2/(E2-D2))</f>
+        <v>-1.0509599527658448E-2</v>
+      </c>
+      <c r="C2" s="24">
+        <f>(F2/(G2-F2))</f>
+        <v>-1.1248402215594375E-2</v>
+      </c>
+      <c r="D2" s="27">
+        <v>-2581</v>
+      </c>
+      <c r="E2" s="27">
+        <v>243004</v>
+      </c>
+      <c r="F2" s="27">
+        <v>-792</v>
+      </c>
+      <c r="G2" s="27">
+        <v>69618</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="20">
+        <v>44995</v>
+      </c>
+      <c r="B3" s="24">
+        <f>(D3/(E3-D3))</f>
+        <v>-9.0863449683541691E-3</v>
+      </c>
+      <c r="C3" s="24">
+        <f>(F3/(G3-F3))</f>
+        <v>-6.20174014174421E-3</v>
+      </c>
+      <c r="D3" s="27">
+        <v>-2208</v>
+      </c>
+      <c r="E3" s="27">
+        <v>240794</v>
+      </c>
+      <c r="F3" s="27">
+        <v>-431.72</v>
+      </c>
+      <c r="G3" s="27">
+        <v>69181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="20">
+        <v>44998</v>
+      </c>
+      <c r="B4" s="24">
+        <f>(D4/(E4-D4))</f>
+        <v>-4.2194793071258169E-3</v>
+      </c>
+      <c r="C4" s="24">
+        <f>(F4/(G4-F4))</f>
+        <v>-4.7279614822954468E-3</v>
+      </c>
+      <c r="D4" s="27">
+        <v>-1017</v>
+      </c>
+      <c r="E4" s="27">
+        <v>240008</v>
+      </c>
+      <c r="F4" s="27">
+        <v>-327</v>
+      </c>
+      <c r="G4" s="27">
+        <v>68836</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="20">
+        <v>44999</v>
+      </c>
+      <c r="B5" s="24">
+        <f>(D5/(E5-D5))</f>
+        <v>7.7849344251381403E-3</v>
+      </c>
+      <c r="C5" s="24">
+        <f>(F5/(G5-F5))</f>
+        <v>-1.394028492554023E-3</v>
+      </c>
+      <c r="D5" s="27">
+        <v>1871</v>
+      </c>
+      <c r="E5" s="27">
+        <v>242207</v>
+      </c>
+      <c r="F5" s="27">
+        <v>-95.99</v>
+      </c>
+      <c r="G5" s="27">
+        <v>68762</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="20">
+        <v>45000</v>
+      </c>
+      <c r="B6" s="24">
+        <f>(D6/(E6-D6))</f>
+        <v>-9.6675750511288835E-3</v>
+      </c>
+      <c r="C6" s="24">
+        <f>(F6/(G6-F6))</f>
+        <v>-9.6527061012661904E-3</v>
+      </c>
+      <c r="D6" s="27">
+        <v>-2341.5500000000002</v>
+      </c>
+      <c r="E6" s="27">
+        <v>239865</v>
+      </c>
+      <c r="F6" s="27">
+        <v>-664</v>
+      </c>
+      <c r="G6" s="27">
+        <v>68125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="20">
+        <v>45001</v>
+      </c>
+      <c r="B7" s="24">
+        <f>(D7/(E7-D7))</f>
+        <v>8.5506430700602425E-3</v>
+      </c>
+      <c r="C7" s="24">
+        <f>(F7/(G7-F7))</f>
+        <v>-8.2764692934184456E-3</v>
+      </c>
+      <c r="D7" s="27">
+        <v>2051</v>
+      </c>
+      <c r="E7" s="27">
+        <v>241916</v>
+      </c>
+      <c r="F7" s="27">
+        <v>-564</v>
+      </c>
+      <c r="G7" s="27">
+        <v>67581</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>